<commit_message>
Making changes for IHS and TCH
</commit_message>
<xml_diff>
--- a/schedules/HIB.xlsx
+++ b/schedules/HIB.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="136">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -401,9 +401,6 @@
     <t>128, 1320, 1330, 1340, 136, 1350, 115, 121, 142, 213</t>
   </si>
   <si>
-    <t>Received 2nd dose at 15 months of age or older, no more doses needed.</t>
-  </si>
-  <si>
     <t>CB</t>
   </si>
   <si>
@@ -432,6 +429,9 @@
   </si>
   <si>
     <t>15 months -4 d</t>
+  </si>
+  <si>
+    <t>Received 2nd dose at 15 months of age or older, one more dose needed.</t>
   </si>
 </sst>
 </file>
@@ -923,6 +923,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -941,24 +944,21 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1472,13 +1472,13 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
@@ -1521,13 +1521,13 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="41"/>
       <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
@@ -1541,9 +1541,9 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="44"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="43"/>
       <c r="F6" s="10" t="s">
         <v>14</v>
       </c>
@@ -1555,13 +1555,13 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="40"/>
+      <c r="D7" s="41"/>
       <c r="F7" s="10" t="s">
         <v>1</v>
       </c>
@@ -1573,9 +1573,9 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="44"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="43"/>
       <c r="F8" s="10" t="s">
         <v>16</v>
       </c>
@@ -1674,11 +1674,11 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
       <c r="F14" s="10" t="s">
         <v>24</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>111</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D16" s="9">
         <v>-7</v>
@@ -1729,7 +1729,7 @@
         <v>110</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D17" s="9">
         <v>-12</v>
@@ -1744,7 +1744,7 @@
         <v>117</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D18" s="9">
         <v>-15</v>
@@ -1944,12 +1944,12 @@
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B63" s="45" t="s">
+      <c r="B63" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="45"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="18"/>
@@ -2034,11 +2034,11 @@
       <c r="E71" s="9"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B72" s="45" t="s">
+      <c r="B72" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="6" t="s">
@@ -2137,12 +2137,12 @@
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B83" s="45" t="s">
+      <c r="B83" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C83" s="45"/>
-      <c r="D83" s="45"/>
-      <c r="E83" s="45"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="39"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B84" s="18"/>
@@ -2229,11 +2229,11 @@
       <c r="E91" s="9"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B92" s="45" t="s">
+      <c r="B92" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C92" s="45"/>
-      <c r="D92" s="45"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="39"/>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B93" s="6" t="s">
@@ -2316,12 +2316,12 @@
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B102" s="45" t="s">
+      <c r="B102" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C102" s="45"/>
-      <c r="D102" s="45"/>
-      <c r="E102" s="45"/>
+      <c r="C102" s="39"/>
+      <c r="D102" s="39"/>
+      <c r="E102" s="39"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B103" s="18"/>
@@ -2408,11 +2408,11 @@
       <c r="E110" s="9"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B111" s="45" t="s">
+      <c r="B111" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C111" s="45"/>
-      <c r="D111" s="45"/>
+      <c r="C111" s="39"/>
+      <c r="D111" s="39"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B112" s="6" t="s">
@@ -2433,7 +2433,7 @@
         <v>110</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D113" s="9"/>
       <c r="E113" s="21" t="s">
@@ -2511,12 +2511,12 @@
       </c>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B122" s="45" t="s">
+      <c r="B122" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C122" s="45"/>
-      <c r="D122" s="45"/>
-      <c r="E122" s="45"/>
+      <c r="C122" s="39"/>
+      <c r="D122" s="39"/>
+      <c r="E122" s="39"/>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B123" s="18"/>
@@ -2603,11 +2603,11 @@
       <c r="E130" s="9"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B131" s="45" t="s">
+      <c r="B131" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C131" s="45"/>
-      <c r="D131" s="45"/>
+      <c r="C131" s="39"/>
+      <c r="D131" s="39"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B132" s="6" t="s">
@@ -2669,12 +2669,12 @@
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B139" s="45" t="s">
+      <c r="B139" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C139" s="45"/>
-      <c r="D139" s="45"/>
-      <c r="E139" s="45"/>
+      <c r="C139" s="39"/>
+      <c r="D139" s="39"/>
+      <c r="E139" s="39"/>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B140" s="18"/>
@@ -2761,11 +2761,11 @@
       <c r="E147" s="9"/>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B148" s="45" t="s">
+      <c r="B148" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C148" s="45"/>
-      <c r="D148" s="45"/>
+      <c r="C148" s="39"/>
+      <c r="D148" s="39"/>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B149" s="6" t="s">
@@ -2790,7 +2790,7 @@
       </c>
       <c r="D150" s="9"/>
       <c r="E150" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.2">
@@ -2851,7 +2851,7 @@
         <v>27</v>
       </c>
       <c r="E157" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.2">
@@ -2863,12 +2863,12 @@
       </c>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B159" s="45" t="s">
+      <c r="B159" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C159" s="45"/>
-      <c r="D159" s="45"/>
-      <c r="E159" s="45"/>
+      <c r="C159" s="39"/>
+      <c r="D159" s="39"/>
+      <c r="E159" s="39"/>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B160" s="18"/>
@@ -2953,11 +2953,11 @@
       <c r="E167" s="9"/>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B168" s="45" t="s">
+      <c r="B168" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C168" s="45"/>
-      <c r="D168" s="45"/>
+      <c r="C168" s="39"/>
+      <c r="D168" s="39"/>
     </row>
     <row r="169" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B169" s="6" t="s">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="D176" s="16"/>
       <c r="E176" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="177" spans="2:5" x14ac:dyDescent="0.2">
@@ -3044,12 +3044,12 @@
       </c>
     </row>
     <row r="178" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B178" s="45" t="s">
+      <c r="B178" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C178" s="45"/>
-      <c r="D178" s="45"/>
-      <c r="E178" s="45"/>
+      <c r="C178" s="39"/>
+      <c r="D178" s="39"/>
+      <c r="E178" s="39"/>
     </row>
     <row r="179" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B179" s="18"/>
@@ -3136,11 +3136,11 @@
       <c r="E186" s="9"/>
     </row>
     <row r="187" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B187" s="45" t="s">
+      <c r="B187" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C187" s="45"/>
-      <c r="D187" s="45"/>
+      <c r="C187" s="39"/>
+      <c r="D187" s="39"/>
     </row>
     <row r="188" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B188" s="6" t="s">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="D189" s="9"/>
       <c r="E189" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="190" spans="2:5" x14ac:dyDescent="0.2">
@@ -3173,11 +3173,11 @@
         <v>13</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D190" s="9"/>
       <c r="E190" s="21" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="191" spans="2:5" x14ac:dyDescent="0.2">
@@ -3230,12 +3230,12 @@
       </c>
     </row>
     <row r="197" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B197" s="45" t="s">
+      <c r="B197" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C197" s="45"/>
-      <c r="D197" s="45"/>
-      <c r="E197" s="45"/>
+      <c r="C197" s="39"/>
+      <c r="D197" s="39"/>
+      <c r="E197" s="39"/>
     </row>
     <row r="198" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B198" s="18"/>
@@ -3307,9 +3307,11 @@
       </c>
       <c r="C204" s="20"/>
       <c r="D204" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E204" s="9"/>
+        <v>40</v>
+      </c>
+      <c r="E204" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="205" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B205" s="19" t="s">
@@ -3320,11 +3322,11 @@
       <c r="E205" s="9"/>
     </row>
     <row r="206" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B206" s="45" t="s">
+      <c r="B206" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C206" s="45"/>
-      <c r="D206" s="45"/>
+      <c r="C206" s="39"/>
+      <c r="D206" s="39"/>
     </row>
     <row r="207" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B207" s="6" t="s">
@@ -3345,11 +3347,11 @@
         <v>117</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D208" s="9"/>
       <c r="E208" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="209" spans="2:5" x14ac:dyDescent="0.2">
@@ -3357,7 +3359,7 @@
         <v>13</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D209" s="9"/>
       <c r="E209" s="21"/>
@@ -3412,24 +3414,24 @@
         <v>27</v>
       </c>
       <c r="E215" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="216" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B216" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C216" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="217" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B217" s="45" t="s">
+      <c r="B217" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C217" s="45"/>
-      <c r="D217" s="45"/>
-      <c r="E217" s="45"/>
+      <c r="C217" s="39"/>
+      <c r="D217" s="39"/>
+      <c r="E217" s="39"/>
     </row>
     <row r="218" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B218" s="18"/>
@@ -3501,9 +3503,11 @@
       </c>
       <c r="C224" s="20"/>
       <c r="D224" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E224" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="E224" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="225" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B225" s="19" t="s">
@@ -3514,11 +3518,11 @@
       <c r="E225" s="9"/>
     </row>
     <row r="226" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B226" s="45" t="s">
+      <c r="B226" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C226" s="45"/>
-      <c r="D226" s="45"/>
+      <c r="C226" s="39"/>
+      <c r="D226" s="39"/>
     </row>
     <row r="227" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B227" s="6" t="s">
@@ -3564,6 +3568,14 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="24">
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B197:E197"/>
+    <mergeCell ref="B187:D187"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="B217:E217"/>
     <mergeCell ref="B226:D226"/>
     <mergeCell ref="F2:J2"/>
@@ -3580,14 +3592,6 @@
     <mergeCell ref="B131:D131"/>
     <mergeCell ref="B148:D148"/>
     <mergeCell ref="B178:E178"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B197:E197"/>
-    <mergeCell ref="B187:D187"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3612,7 +3616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A129"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection sqref="A1:A129"/>
     </sheetView>
   </sheetViews>
@@ -4224,7 +4228,7 @@
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="23" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B190&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C190&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D190&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E190&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="Series Dose" schedule="P4" age="" reason="Received 2nd dose at 15 months of age or older, no more doses needed."/&gt;</v>
+        <v xml:space="preserve">    &lt;indicate vaccineName="Series Dose" schedule="CB" age="" reason="Received 2nd dose at 15 months of age or older, one more dose needed."/&gt;</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
@@ -4284,7 +4288,7 @@
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="23" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D204&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E204&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
+        <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
@@ -4368,7 +4372,7 @@
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="23" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D224&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E224&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
+        <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
@@ -4433,42 +4437,42 @@
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
       <c r="J3" s="46" t="s">
         <v>29</v>
       </c>
       <c r="K3" s="46"/>
       <c r="L3" s="46"/>
       <c r="M3" s="46"/>
-      <c r="N3" s="47" t="s">
+      <c r="N3" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
       <c r="R3" s="46" t="s">
         <v>30</v>
       </c>
       <c r="S3" s="46"/>
       <c r="T3" s="46"/>
       <c r="U3" s="46"/>
-      <c r="V3" s="55" t="s">
+      <c r="V3" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="W3" s="55"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="49" t="s">
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49"/>
+      <c r="AA3" s="50"/>
+      <c r="AB3" s="50"/>
+      <c r="AC3" s="50"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B4" s="25"/>
@@ -4501,62 +4505,62 @@
       <c r="AC4" s="29"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="H5" s="50" t="s">
+      <c r="H5" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="50"/>
-      <c r="AC5" s="50"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="52"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52"/>
+      <c r="X5" s="52"/>
+      <c r="Y5" s="52"/>
+      <c r="Z5" s="52"/>
+      <c r="AA5" s="52"/>
+      <c r="AB5" s="52"/>
+      <c r="AC5" s="52"/>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="H7" s="51" t="s">
+      <c r="H7" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="52" t="s">
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="53" t="s">
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="52" t="s">
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="56"/>
+      <c r="T7" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="54" t="s">
+      <c r="U7" s="55"/>
+      <c r="V7" s="55"/>
+      <c r="W7" s="55"/>
+      <c r="X7" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="Y7" s="54"/>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="54"/>
+      <c r="Y7" s="57"/>
+      <c r="Z7" s="57"/>
+      <c r="AA7" s="57"/>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.2">
       <c r="H8" s="30"/>
@@ -4581,48 +4585,48 @@
       <c r="AA8" s="29"/>
     </row>
     <row r="9" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="H9" s="50" t="s">
+      <c r="H9" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="50"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="50"/>
-      <c r="U9" s="50"/>
-      <c r="V9" s="50"/>
-      <c r="W9" s="50"/>
-      <c r="X9" s="50"/>
-      <c r="Y9" s="50"/>
-      <c r="Z9" s="50"/>
-      <c r="AA9" s="50"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="52"/>
+      <c r="V9" s="52"/>
+      <c r="W9" s="52"/>
+      <c r="X9" s="52"/>
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="52"/>
+      <c r="AA9" s="52"/>
     </row>
     <row r="11" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="57" t="s">
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="58" t="s">
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="58"/>
-      <c r="S11" s="58"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="60"/>
+      <c r="S11" s="60"/>
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.2">
       <c r="H12" s="30"/>
@@ -4639,38 +4643,38 @@
       <c r="S12" s="29"/>
     </row>
     <row r="13" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="H13" s="50" t="s">
+      <c r="H13" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="52"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="H15" s="48" t="s">
+      <c r="H15" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48" t="s">
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="48"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="53"/>
+      <c r="R15" s="53"/>
+      <c r="S15" s="53"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="H16" s="30"/>
@@ -4687,20 +4691,20 @@
       <c r="S16" s="29"/>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="H17" s="50" t="s">
+      <c r="H17" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="50"/>
-      <c r="P17" s="50"/>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="50"/>
-      <c r="S17" s="50"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="52"/>
     </row>
     <row r="23" spans="2:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
@@ -4714,42 +4718,42 @@
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
       <c r="E25" s="46"/>
-      <c r="F25" s="47" t="s">
+      <c r="F25" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
       <c r="J25" s="46" t="s">
         <v>29</v>
       </c>
       <c r="K25" s="46"/>
       <c r="L25" s="46"/>
       <c r="M25" s="46"/>
-      <c r="N25" s="47" t="s">
+      <c r="N25" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="O25" s="47"/>
-      <c r="P25" s="47"/>
-      <c r="Q25" s="47"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="48"/>
+      <c r="Q25" s="48"/>
       <c r="R25" s="46" t="s">
         <v>30</v>
       </c>
       <c r="S25" s="46"/>
       <c r="T25" s="46"/>
       <c r="U25" s="46"/>
-      <c r="V25" s="55" t="s">
+      <c r="V25" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="W25" s="55"/>
-      <c r="X25" s="55"/>
-      <c r="Y25" s="55"/>
-      <c r="Z25" s="49" t="s">
+      <c r="W25" s="49"/>
+      <c r="X25" s="49"/>
+      <c r="Y25" s="49"/>
+      <c r="Z25" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="AA25" s="49"/>
-      <c r="AB25" s="49"/>
-      <c r="AC25" s="49"/>
+      <c r="AA25" s="50"/>
+      <c r="AB25" s="50"/>
+      <c r="AC25" s="50"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B26" s="25"/>
@@ -4782,14 +4786,14 @@
       <c r="AC26" s="29"/>
     </row>
     <row r="29" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
       <c r="H29" s="31"/>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -4826,24 +4830,24 @@
       <c r="I32" s="46"/>
       <c r="J32" s="46"/>
       <c r="K32" s="46"/>
-      <c r="L32" s="47" t="s">
+      <c r="L32" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="48"/>
       <c r="P32" s="46" t="s">
         <v>29</v>
       </c>
       <c r="Q32" s="46"/>
       <c r="R32" s="46"/>
       <c r="S32" s="46"/>
-      <c r="T32" s="60" t="s">
+      <c r="T32" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="U32" s="60"/>
-      <c r="V32" s="60"/>
-      <c r="W32" s="60"/>
+      <c r="U32" s="47"/>
+      <c r="V32" s="47"/>
+      <c r="W32" s="47"/>
     </row>
     <row r="33" spans="6:33" x14ac:dyDescent="0.2">
       <c r="G33" s="35" t="s">
@@ -4904,24 +4908,24 @@
       <c r="K37" s="46"/>
       <c r="L37" s="46"/>
       <c r="M37" s="46"/>
-      <c r="N37" s="47" t="s">
+      <c r="N37" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="O37" s="47"/>
-      <c r="P37" s="47"/>
-      <c r="Q37" s="47"/>
+      <c r="O37" s="48"/>
+      <c r="P37" s="48"/>
+      <c r="Q37" s="48"/>
       <c r="R37" s="46" t="s">
         <v>29</v>
       </c>
       <c r="S37" s="46"/>
       <c r="T37" s="46"/>
       <c r="U37" s="46"/>
-      <c r="V37" s="60" t="s">
+      <c r="V37" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="W37" s="60"/>
-      <c r="X37" s="60"/>
-      <c r="Y37" s="60"/>
+      <c r="W37" s="47"/>
+      <c r="X37" s="47"/>
+      <c r="Y37" s="47"/>
     </row>
     <row r="38" spans="6:33" x14ac:dyDescent="0.2">
       <c r="I38" s="35" t="s">
@@ -4982,24 +4986,24 @@
       <c r="O42" s="46"/>
       <c r="P42" s="46"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="47" t="s">
+      <c r="R42" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="S42" s="47"/>
-      <c r="T42" s="47"/>
-      <c r="U42" s="47"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="48"/>
+      <c r="U42" s="48"/>
       <c r="V42" s="46" t="s">
         <v>29</v>
       </c>
       <c r="W42" s="46"/>
       <c r="X42" s="46"/>
       <c r="Y42" s="46"/>
-      <c r="Z42" s="60" t="s">
+      <c r="Z42" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="AA42" s="60"/>
-      <c r="AB42" s="60"/>
-      <c r="AC42" s="60"/>
+      <c r="AA42" s="47"/>
+      <c r="AB42" s="47"/>
+      <c r="AC42" s="47"/>
     </row>
     <row r="43" spans="6:33" x14ac:dyDescent="0.2">
       <c r="M43" s="35" t="s">
@@ -5060,24 +5064,24 @@
       <c r="S47" s="46"/>
       <c r="T47" s="46"/>
       <c r="U47" s="46"/>
-      <c r="V47" s="47" t="s">
+      <c r="V47" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="W47" s="47"/>
-      <c r="X47" s="47"/>
-      <c r="Y47" s="47"/>
+      <c r="W47" s="48"/>
+      <c r="X47" s="48"/>
+      <c r="Y47" s="48"/>
       <c r="Z47" s="46" t="s">
         <v>29</v>
       </c>
       <c r="AA47" s="46"/>
       <c r="AB47" s="46"/>
       <c r="AC47" s="46"/>
-      <c r="AD47" s="60" t="s">
+      <c r="AD47" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="AE47" s="60"/>
-      <c r="AF47" s="60"/>
-      <c r="AG47" s="60"/>
+      <c r="AE47" s="47"/>
+      <c r="AF47" s="47"/>
+      <c r="AG47" s="47"/>
     </row>
     <row r="48" spans="6:33" x14ac:dyDescent="0.2">
       <c r="Q48" s="35" t="s">
@@ -5138,24 +5142,24 @@
       <c r="I52" s="46"/>
       <c r="J52" s="46"/>
       <c r="K52" s="46"/>
-      <c r="L52" s="47" t="s">
+      <c r="L52" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="M52" s="47"/>
-      <c r="N52" s="47"/>
-      <c r="O52" s="47"/>
+      <c r="M52" s="48"/>
+      <c r="N52" s="48"/>
+      <c r="O52" s="48"/>
       <c r="P52" s="46" t="s">
         <v>29</v>
       </c>
       <c r="Q52" s="46"/>
       <c r="R52" s="46"/>
       <c r="S52" s="46"/>
-      <c r="T52" s="60" t="s">
+      <c r="T52" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="U52" s="60"/>
-      <c r="V52" s="60"/>
-      <c r="W52" s="60"/>
+      <c r="U52" s="47"/>
+      <c r="V52" s="47"/>
+      <c r="W52" s="47"/>
     </row>
     <row r="53" spans="4:33" x14ac:dyDescent="0.2">
       <c r="G53" s="35" t="s">
@@ -5220,24 +5224,24 @@
       <c r="K57" s="46"/>
       <c r="L57" s="46"/>
       <c r="M57" s="46"/>
-      <c r="N57" s="47" t="s">
+      <c r="N57" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="O57" s="47"/>
-      <c r="P57" s="47"/>
-      <c r="Q57" s="47"/>
+      <c r="O57" s="48"/>
+      <c r="P57" s="48"/>
+      <c r="Q57" s="48"/>
       <c r="R57" s="46" t="s">
         <v>29</v>
       </c>
       <c r="S57" s="46"/>
       <c r="T57" s="46"/>
       <c r="U57" s="46"/>
-      <c r="V57" s="60" t="s">
+      <c r="V57" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="W57" s="60"/>
-      <c r="X57" s="60"/>
-      <c r="Y57" s="60"/>
+      <c r="W57" s="47"/>
+      <c r="X57" s="47"/>
+      <c r="Y57" s="47"/>
     </row>
     <row r="58" spans="4:33" x14ac:dyDescent="0.2">
       <c r="I58" s="35" t="s">
@@ -5302,24 +5306,24 @@
       <c r="S62" s="46"/>
       <c r="T62" s="46"/>
       <c r="U62" s="46"/>
-      <c r="V62" s="47" t="s">
+      <c r="V62" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="W62" s="47"/>
-      <c r="X62" s="47"/>
-      <c r="Y62" s="47"/>
+      <c r="W62" s="48"/>
+      <c r="X62" s="48"/>
+      <c r="Y62" s="48"/>
       <c r="Z62" s="46" t="s">
         <v>29</v>
       </c>
       <c r="AA62" s="46"/>
       <c r="AB62" s="46"/>
       <c r="AC62" s="46"/>
-      <c r="AD62" s="60" t="s">
+      <c r="AD62" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="AE62" s="60"/>
-      <c r="AF62" s="60"/>
-      <c r="AG62" s="60"/>
+      <c r="AE62" s="47"/>
+      <c r="AF62" s="47"/>
+      <c r="AG62" s="47"/>
     </row>
     <row r="63" spans="4:33" x14ac:dyDescent="0.2">
       <c r="Q63" s="35" t="s">
@@ -5374,43 +5378,11 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="57">
-    <mergeCell ref="Z62:AC62"/>
-    <mergeCell ref="AD62:AG62"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="N57:Q57"/>
-    <mergeCell ref="R57:U57"/>
-    <mergeCell ref="V57:Y57"/>
-    <mergeCell ref="R62:U62"/>
-    <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="Z42:AC42"/>
-    <mergeCell ref="R47:U47"/>
-    <mergeCell ref="V47:Y47"/>
-    <mergeCell ref="Z47:AC47"/>
-    <mergeCell ref="AD47:AG47"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="L52:O52"/>
-    <mergeCell ref="P52:S52"/>
-    <mergeCell ref="T52:W52"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="N37:Q37"/>
-    <mergeCell ref="R37:U37"/>
-    <mergeCell ref="V37:Y37"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="V25:Y25"/>
-    <mergeCell ref="Z25:AC25"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="L32:O32"/>
-    <mergeCell ref="P32:S32"/>
-    <mergeCell ref="T32:W32"/>
-    <mergeCell ref="H17:S17"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="R25:U25"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="L15:S15"/>
     <mergeCell ref="Z3:AC3"/>
@@ -5426,11 +5398,43 @@
     <mergeCell ref="L11:O11"/>
     <mergeCell ref="P11:S11"/>
     <mergeCell ref="H13:S13"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="H17:S17"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="R25:U25"/>
+    <mergeCell ref="V25:Y25"/>
+    <mergeCell ref="Z25:AC25"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="L32:O32"/>
+    <mergeCell ref="P32:S32"/>
+    <mergeCell ref="T32:W32"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:O52"/>
+    <mergeCell ref="P52:S52"/>
+    <mergeCell ref="T52:W52"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="N37:Q37"/>
+    <mergeCell ref="R37:U37"/>
+    <mergeCell ref="V37:Y37"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="Z42:AC42"/>
+    <mergeCell ref="R47:U47"/>
+    <mergeCell ref="V47:Y47"/>
+    <mergeCell ref="Z47:AC47"/>
+    <mergeCell ref="AD47:AG47"/>
+    <mergeCell ref="Z62:AC62"/>
+    <mergeCell ref="AD62:AG62"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="N57:Q57"/>
+    <mergeCell ref="R57:U57"/>
+    <mergeCell ref="V57:Y57"/>
+    <mergeCell ref="R62:U62"/>
+    <mergeCell ref="V62:Y62"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0263888888888888" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>